<commit_message>
user input for year, picking schools data from previous year sheet.
</commit_message>
<xml_diff>
--- a/AllocationCalculator/Content/Uploads/h sheet.xlsx
+++ b/AllocationCalculator/Content/Uploads/h sheet.xlsx
@@ -631,7 +631,7 @@
   <dimension ref="A1:AF23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1284,19 +1284,10 @@
       <c r="F22" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="G22" s="65">
-        <v>176540.50391487594</v>
-      </c>
-      <c r="H22" s="64">
-        <v>2441</v>
-      </c>
-      <c r="I22" s="57">
-        <f t="shared" ref="I22:I23" si="1">(G22-H22)</f>
-        <v>174099.50391487594</v>
-      </c>
-      <c r="J22" s="66">
-        <v>204863.27976810708</v>
-      </c>
+      <c r="G22" s="65"/>
+      <c r="H22" s="64"/>
+      <c r="I22" s="57"/>
+      <c r="J22" s="66"/>
       <c r="K22" s="48"/>
       <c r="L22" s="48"/>
       <c r="M22" s="49"/>
@@ -1339,19 +1330,10 @@
       <c r="F23" s="54" t="s">
         <v>6</v>
       </c>
-      <c r="G23" s="65">
-        <v>471121.02052754903</v>
-      </c>
-      <c r="H23" s="64">
-        <v>0</v>
-      </c>
-      <c r="I23" s="57">
-        <f t="shared" si="1"/>
-        <v>471121.02052754903</v>
-      </c>
-      <c r="J23" s="66">
-        <v>432652.86429048353</v>
-      </c>
+      <c r="G23" s="65"/>
+      <c r="H23" s="64"/>
+      <c r="I23" s="57"/>
+      <c r="J23" s="66"/>
       <c r="K23" s="48"/>
       <c r="L23" s="48"/>
       <c r="M23" s="49"/>

</xml_diff>